<commit_message>
Added rounding out decimals functionality
</commit_message>
<xml_diff>
--- a/Watson-data.xlsx
+++ b/Watson-data.xlsx
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BP7" sqref="BP7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3715,6 +3715,165 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
+      <c r="I15">
+        <v>2653</v>
+      </c>
+      <c r="K15">
+        <v>97</v>
+      </c>
+      <c r="L15">
+        <v>98</v>
+      </c>
+      <c r="M15">
+        <v>93</v>
+      </c>
+      <c r="N15">
+        <v>90</v>
+      </c>
+      <c r="O15">
+        <v>60</v>
+      </c>
+      <c r="P15">
+        <v>15</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>94</v>
+      </c>
+      <c r="S15">
+        <v>8</v>
+      </c>
+      <c r="T15">
+        <v>15</v>
+      </c>
+      <c r="U15">
+        <v>7</v>
+      </c>
+      <c r="V15">
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <v>3</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>87</v>
+      </c>
+      <c r="Z15">
+        <v>99</v>
+      </c>
+      <c r="AA15">
+        <v>91</v>
+      </c>
+      <c r="AB15">
+        <v>87</v>
+      </c>
+      <c r="AC15">
+        <v>85</v>
+      </c>
+      <c r="AD15">
+        <v>66</v>
+      </c>
+      <c r="AE15">
+        <v>34</v>
+      </c>
+      <c r="AF15">
+        <v>84</v>
+      </c>
+      <c r="AG15">
+        <v>98</v>
+      </c>
+      <c r="AH15">
+        <v>96</v>
+      </c>
+      <c r="AI15">
+        <v>89</v>
+      </c>
+      <c r="AJ15">
+        <v>40</v>
+      </c>
+      <c r="AK15">
+        <v>33</v>
+      </c>
+      <c r="AL15">
+        <v>2</v>
+      </c>
+      <c r="AM15">
+        <v>19</v>
+      </c>
+      <c r="AN15">
+        <v>94</v>
+      </c>
+      <c r="AO15">
+        <v>67</v>
+      </c>
+      <c r="AP15">
+        <v>96</v>
+      </c>
+      <c r="AQ15">
+        <v>97</v>
+      </c>
+      <c r="AR15">
+        <v>85</v>
+      </c>
+      <c r="AS15">
+        <v>34</v>
+      </c>
+      <c r="AT15">
+        <v>21</v>
+      </c>
+      <c r="AU15">
+        <v>40</v>
+      </c>
+      <c r="AV15">
+        <v>3</v>
+      </c>
+      <c r="AW15">
+        <v>6</v>
+      </c>
+      <c r="AX15">
+        <v>4</v>
+      </c>
+      <c r="AY15">
+        <v>12</v>
+      </c>
+      <c r="AZ15">
+        <v>8</v>
+      </c>
+      <c r="BA15">
+        <v>3</v>
+      </c>
+      <c r="BB15">
+        <v>5</v>
+      </c>
+      <c r="BC15">
+        <v>3</v>
+      </c>
+      <c r="BD15">
+        <v>1</v>
+      </c>
+      <c r="BE15">
+        <v>3</v>
+      </c>
+      <c r="BF15">
+        <v>36</v>
+      </c>
+      <c r="BG15">
+        <v>4</v>
+      </c>
+      <c r="BH15">
+        <v>3</v>
+      </c>
+      <c r="BI15">
+        <v>3</v>
+      </c>
+      <c r="BJ15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.55000000000000004">
       <c r="F16" s="1"/>

</xml_diff>